<commit_message>
feat: Add company admin overview page and update data manage overview page
</commit_message>
<xml_diff>
--- a/config/system_permission.xlsx
+++ b/config/system_permission.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yahoo168/Desktop/alphahelix-internal-system/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA23AA1-402F-3046-B63C-AD752868F8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B661A9-1F0A-3E48-9459-A7731A8FE0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6220" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{51010CA0-E2AE-4344-B7E3-E191DA907A24}"/>
   </bookViews>
@@ -267,7 +267,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -294,13 +294,6 @@
       <sz val="9"/>
       <name val="Wawati TC"/>
       <family val="3"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color rgb="FFFF0000"/>
-      <name val="微軟正黑體"/>
-      <family val="2"/>
       <charset val="136"/>
     </font>
     <font>
@@ -382,24 +375,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -750,29 +740,28 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
     <col min="6" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5" customWidth="1"/>
+    <col min="10" max="11" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="22">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -807,36 +796,36 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="69">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="6" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1014,7 +1003,7 @@
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1040,7 +1029,7 @@
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1066,7 +1055,7 @@
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C11" s="2"/>
@@ -1086,7 +1075,7 @@
       <c r="A12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>41</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1112,7 +1101,7 @@
       <c r="A13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1138,7 +1127,7 @@
       <c r="A14" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="2"/>
@@ -1175,10 +1164,10 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="22">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="9"/>
+      <c r="B17" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1203,34 +1192,34 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10" ht="92">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>